<commit_message>
Se agrega sript para cálculo de parámetros. Se nota que queda de baja resolución el parámetro K_Ts que depende de la frecuencia de muestreo. Se hace commit para registrar cambios en versión nueva.
</commit_message>
<xml_diff>
--- a/doc/tuning_params_motor_bt2.xlsx
+++ b/doc/tuning_params_motor_bt2.xlsx
@@ -200,7 +200,13 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -218,33 +224,33 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -252,6 +258,28 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -259,67 +287,48 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -327,11 +336,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -340,30 +351,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -381,6 +368,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -432,7 +443,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -456,55 +467,52 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -513,59 +521,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,7 +581,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -589,7 +597,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,59 +617,58 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
+    <cellStyle name="Accent 1 14" xfId="20"/>
+    <cellStyle name="Accent 13" xfId="21"/>
+    <cellStyle name="Accent 2 15" xfId="22"/>
+    <cellStyle name="Accent 3 16" xfId="23"/>
+    <cellStyle name="Bad 10" xfId="24"/>
+    <cellStyle name="Error 12" xfId="25"/>
+    <cellStyle name="Footnote 5" xfId="26"/>
+    <cellStyle name="Good 8" xfId="27"/>
+    <cellStyle name="Heading 1 1" xfId="28"/>
+    <cellStyle name="Heading 2 2" xfId="29"/>
+    <cellStyle name="Hyperlink 6" xfId="30"/>
+    <cellStyle name="Neutral 9" xfId="31"/>
+    <cellStyle name="Note 4" xfId="32"/>
+    <cellStyle name="Status 7" xfId="33"/>
+    <cellStyle name="Text 3" xfId="34"/>
+    <cellStyle name="Warning 11" xfId="35"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -734,7 +741,7 @@
   <dimension ref="A1:N170"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L28" activeCellId="0" sqref="L28"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -749,7 +756,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.42"/>
   </cols>
   <sheetData>

</xml_diff>